<commit_message>
bug fix to reg_RSME.xlsx + update to POM for new jasmine-core
</commit_message>
<xml_diff>
--- a/input/EUROMODpolicySchedule.xlsx
+++ b/input/EUROMODpolicySchedule.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17032" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17100" uniqueCount="61">
   <si>
     <t>Filename</t>
   </si>
@@ -685,7 +685,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC6207-DD24-427A-A7C5-E1B68985A6D0}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -713,13 +713,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -727,13 +727,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -741,13 +741,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -755,13 +755,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -769,13 +769,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -783,13 +783,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
@@ -797,13 +797,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -811,13 +811,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -825,13 +825,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -839,13 +839,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -853,13 +853,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -867,13 +867,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -895,13 +895,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
@@ -909,13 +909,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
@@ -923,71 +923,15 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced orphan error with warning message
</commit_message>
<xml_diff>
--- a/input/EUROMODpolicySchedule.xlsx
+++ b/input/EUROMODpolicySchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\labsim_Italy\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CE18F5-E866-417E-9A4C-21A199A848C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F0610D-9867-49D9-9F5B-A4E2213BB68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="20400" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17312" uniqueCount="61">
   <si>
     <t>Filename</t>
   </si>
@@ -49,6 +49,9 @@
     <t>it_2015_std.txt</t>
   </si>
   <si>
+    <t>2017</t>
+  </si>
+  <si>
     <t>2019</t>
   </si>
   <si>
@@ -58,6 +61,21 @@
     <t>2020</t>
   </si>
   <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
     <t>Policy for 2015</t>
   </si>
   <si>
@@ -85,54 +103,36 @@
     <t>uk_2019_std.txt</t>
   </si>
   <si>
+    <t>uk_2011_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2012_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2013_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2014_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2017_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2018_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2020_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2021_std.txt</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
     <t>Policy_System_Year</t>
   </si>
   <si>
-    <t>uk_2011_std.txt</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>uk_2012_std.txt</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>uk_2013_std.txt</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>uk_2014_std.txt</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>uk_2017_std.txt</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>uk_2018_std.txt</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>uk_2020_std.txt</t>
-  </si>
-  <si>
-    <t>uk_2021_std.txt</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
     <t>uk_2022_std.txt</t>
   </si>
   <si>
@@ -151,6 +151,54 @@
     <t>2024</t>
   </si>
   <si>
+    <t>uk_2021_10_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2022_10_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2023_10_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2024_10_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2010_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2017_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2018_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2019_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2020_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2021_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2022_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2023_std.txt</t>
+  </si>
+  <si>
+    <t>hscl_uk_2024_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2022_nohscl_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2023_nohscl_std.txt</t>
+  </si>
+  <si>
+    <t>uk_2024_nohscl_std.txt</t>
+  </si>
+  <si>
     <t>uk_2025_std.txt</t>
   </si>
   <si>
@@ -161,12 +209,6 @@
   </si>
   <si>
     <t>2026</t>
-  </si>
-  <si>
-    <t>uk_2027_std.txt</t>
-  </si>
-  <si>
-    <t>2027</t>
   </si>
 </sst>
 </file>
@@ -223,9 +265,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,7 +305,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -369,7 +411,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -511,7 +553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,18 +563,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="1026" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="1026" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,13 +583,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -554,10 +597,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -565,73 +608,73 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -642,14 +685,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC6207-DD24-427A-A7C5-E1B68985A6D0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="2" max="1025" width="9.1796875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="1025" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -660,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -668,63 +713,63 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -733,12 +778,12 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -747,21 +792,21 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -769,55 +814,55 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -831,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -845,7 +890,7 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -859,49 +904,35 @@
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix problem with training data
</commit_message>
<xml_diff>
--- a/input/EUROMODpolicySchedule.xlsx
+++ b/input/EUROMODpolicySchedule.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17384" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17312" uniqueCount="61">
   <si>
     <t>Filename</t>
   </si>
@@ -209,12 +209,6 @@
   </si>
   <si>
     <t>2026</t>
-  </si>
-  <si>
-    <t>uk_2027_std.txt</t>
-  </si>
-  <si>
-    <t>2027</t>
   </si>
 </sst>
 </file>
@@ -691,7 +685,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC6207-DD24-427A-A7C5-E1B68985A6D0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -941,20 +935,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
remove 2027 from file to stop failing first runs
</commit_message>
<xml_diff>
--- a/input/EUROMODpolicySchedule.xlsx
+++ b/input/EUROMODpolicySchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\EUROMODoutput\current\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\temp\SimPaths_other\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3402BA8E-92CD-40B8-B77E-691FC16035DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F34954F-FC78-4AC0-9B45-2944A0046402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
   <si>
     <t>Filename</t>
   </si>
@@ -161,19 +161,12 @@
   </si>
   <si>
     <t>2026</t>
-  </si>
-  <si>
-    <t>uk_2027_std.txt</t>
-  </si>
-  <si>
-    <t>2027</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:AML9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -527,9 +520,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="1026" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="1026" width="8.7109375" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,19 +635,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC6207-DD24-427A-A7C5-E1B68985A6D0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="1025" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="1025" width="9.140625" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -682,7 +675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -696,7 +689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -710,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -724,7 +717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -738,7 +731,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -752,7 +745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -766,7 +759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -780,7 +773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -794,7 +787,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -808,7 +801,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -822,7 +815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -836,7 +829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -850,7 +843,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -864,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -878,7 +871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -892,16 +885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
add test routine for regression models and revert experimental regression estimates
</commit_message>
<xml_diff>
--- a/input/EUROMODpolicySchedule.xlsx
+++ b/input/EUROMODpolicySchedule.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="47">
   <si>
     <t>Filename</t>
   </si>
@@ -642,7 +642,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC6207-DD24-427A-A7C5-E1B68985A6D0}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -670,13 +670,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -684,225 +684,15 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug in parameters
</commit_message>
<xml_diff>
--- a/input/EUROMODpolicySchedule.xlsx
+++ b/input/EUROMODpolicySchedule.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="47">
   <si>
     <t>Filename</t>
   </si>
@@ -642,7 +642,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC6207-DD24-427A-A7C5-E1B68985A6D0}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -670,13 +670,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -684,15 +684,211 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>